<commit_message>
Updated to bloodmeal_euks for new LCA
</commit_message>
<xml_diff>
--- a/figures/fig4/bloodmeal_parasites.xlsx
+++ b/figures/fig4/bloodmeal_parasites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanna/Desktop/MyBox/aa_DeRisi/mosquito/2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FB29EA-CA7E-DE46-A9A6-202A79495202}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CE62F0-9CB8-244A-A789-886BC59647E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{45CD69A5-225C-F841-94BF-9281A83BE651}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="254">
   <si>
     <t>CMS001_040_Ra_S21</t>
   </si>
@@ -105,9 +105,6 @@
     <t>NODE_1435_length_396_cov_300.821317</t>
   </si>
   <si>
-    <t>NODE_1125_length_443_cov_118.942623</t>
-  </si>
-  <si>
     <t>NODE_2444_length_311_cov_183.658120</t>
   </si>
   <si>
@@ -141,9 +138,6 @@
     <t>NODE_1926_length_350_cov_0.802198</t>
   </si>
   <si>
-    <t>NODE_2251_length_325_cov_0.794355</t>
-  </si>
-  <si>
     <t>NODE_2387_length_315_cov_1.529412</t>
   </si>
   <si>
@@ -879,9 +873,6 @@
     <t>JN006842.1</t>
   </si>
   <si>
-    <t>CP015675.1</t>
-  </si>
-  <si>
     <t>MK516192.1</t>
   </si>
   <si>
@@ -918,12 +909,6 @@
     <t>XM_015802553.1</t>
   </si>
   <si>
-    <t>BK010874.1</t>
-  </si>
-  <si>
-    <t>Endotrypanum schaudinni </t>
-  </si>
-  <si>
     <t>XM_015799557.1</t>
   </si>
   <si>
@@ -1124,9 +1109,6 @@
     <t>Invertebrates (monoxenous)</t>
   </si>
   <si>
-    <t>Sloths (dixenous)</t>
-  </si>
-  <si>
     <t>Mammals, lizards (dixenous)</t>
   </si>
   <si>
@@ -1205,13 +1187,73 @@
   </si>
   <si>
     <t>Deer</t>
+  </si>
+  <si>
+    <t>XM_015805759.1</t>
+  </si>
+  <si>
+    <t>NODE_2105_length_313_cov_0.927966</t>
+  </si>
+  <si>
+    <t>XM_015796546.1</t>
+  </si>
+  <si>
+    <t>XM_015796549.1</t>
+  </si>
+  <si>
+    <t>XM_015802014.1</t>
+  </si>
+  <si>
+    <t>KT944293.1</t>
+  </si>
+  <si>
+    <t>Trypanosomatidae sp.</t>
+  </si>
+  <si>
+    <t>XM_003877341.1</t>
+  </si>
+  <si>
+    <t>Leishmania mexicana</t>
+  </si>
+  <si>
+    <t>XM_015798305.1</t>
+  </si>
+  <si>
+    <t>XR_001548769.1</t>
+  </si>
+  <si>
+    <t>XM_801183.1</t>
+  </si>
+  <si>
+    <t>NODE_806_length_317_cov_1.000000</t>
+  </si>
+  <si>
+    <t>NODE_1340_length_268_cov_1.513089</t>
+  </si>
+  <si>
+    <t>NODE_2166_length_331_cov_0.755906</t>
+  </si>
+  <si>
+    <t>NODE_2521_length_306_cov_0.772926</t>
+  </si>
+  <si>
+    <t>NODE_4268_length_257_cov_3.572222</t>
+  </si>
+  <si>
+    <t>NODE_5956_length_230_cov_1.431373</t>
+  </si>
+  <si>
+    <t>NODE_1133_length_282_cov_1.424390</t>
+  </si>
+  <si>
+    <t>NODE_1219_length_277_cov_1.460000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1237,13 +1279,6 @@
     </font>
     <font>
       <i/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1287,7 +1322,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1309,6 +1344,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1624,7 +1663,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B35D40C4-295E-1D4F-8EBF-73F91F32C44C}">
-  <dimension ref="A1:H87"/>
+  <dimension ref="A1:H94"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
   </sheetViews>
@@ -1642,163 +1681,163 @@
   <sheetData>
     <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>238</v>
-      </c>
       <c r="G2" s="18" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="G3" s="18" t="s">
         <v>233</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>239</v>
-      </c>
       <c r="H3" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C6" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="E6" s="19" t="s">
         <v>231</v>
       </c>
-      <c r="D6" s="17" t="s">
-        <v>236</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>237</v>
-      </c>
       <c r="F6" s="19" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="H6" s="19" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>8</v>
@@ -1807,22 +1846,22 @@
         <v>9</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>10</v>
@@ -1831,24 +1870,24 @@
         <v>11</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>10</v>
@@ -1857,24 +1896,24 @@
         <v>12</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>13</v>
@@ -1883,22 +1922,22 @@
         <v>14</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>0</v>
@@ -1907,22 +1946,22 @@
         <v>3</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>0</v>
@@ -1931,22 +1970,22 @@
         <v>1</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>0</v>
@@ -1955,22 +1994,22 @@
         <v>4</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>0</v>
@@ -1979,24 +2018,24 @@
         <v>2</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>5</v>
@@ -2005,22 +2044,22 @@
         <v>7</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>5</v>
@@ -2029,384 +2068,384 @@
         <v>6</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G16" s="10"/>
       <c r="H16" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="D18" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B23" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C24" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>110</v>
+      <c r="D25" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="6" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>138</v>
-      </c>
       <c r="E27" s="9" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="6" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>127</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="F28" s="6"/>
       <c r="G28" s="6" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>110</v>
+      <c r="A29" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="D30" s="5" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>208</v>
+        <v>120</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>159</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>129</v>
@@ -2414,681 +2453,679 @@
       <c r="E31" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="F31" s="1"/>
+      <c r="F31" s="1" t="s">
+        <v>203</v>
+      </c>
       <c r="G31" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D33" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>113</v>
+      <c r="E34" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>113</v>
+      <c r="A35" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="H36" s="6" t="s">
-        <v>113</v>
+      <c r="A36" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D36" s="22" t="s">
+        <v>237</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B38" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C38" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C38" s="6" t="s">
-        <v>81</v>
-      </c>
       <c r="D38" s="8" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="E38" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D41" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="F38" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="H38" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="E40" s="2" t="s">
+      <c r="E41" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F41" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="G40" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>113</v>
+      <c r="G41" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>83</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="F42" s="1"/>
+        <v>147</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="G42" s="1" t="s">
-        <v>223</v>
+        <v>204</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="D43" s="5" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="F44" s="9"/>
-      <c r="G44" s="6" t="s">
+      <c r="A44" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G44" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="H44" s="6" t="s">
-        <v>110</v>
+      <c r="H44" s="1" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="F45" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="G45" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="H45" s="6" t="s">
-        <v>110</v>
+      <c r="A45" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="E46" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="H46" s="6" t="s">
-        <v>110</v>
+      <c r="A46" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>179</v>
+        <v>138</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="F47" s="9" t="s">
-        <v>202</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="F47" s="9"/>
       <c r="G47" s="6" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>187</v>
+        <v>136</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="F48" s="9" t="s">
-        <v>205</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="F48" s="6"/>
       <c r="G48" s="6" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>184</v>
+        <v>147</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>223</v>
+        <v>204</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="F50" s="9" t="s">
         <v>200</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>225</v>
+        <v>204</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>132</v>
+        <v>181</v>
       </c>
       <c r="F51" s="9" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>132</v>
+        <v>175</v>
       </c>
       <c r="F52" s="9" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>151</v>
+        <v>189</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="F53" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>190</v>
+        <v>130</v>
       </c>
       <c r="F54" s="9" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>183</v>
+        <v>149</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>184</v>
+        <v>147</v>
       </c>
       <c r="F55" s="9" t="s">
-        <v>161</v>
+        <v>197</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>223</v>
+        <v>204</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="E56" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="F56" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="F56" s="9"/>
       <c r="G56" s="6" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H56" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B57" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B57" s="23" t="s">
         <v>10</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D57" s="8" t="s">
-        <v>195</v>
+        <v>248</v>
+      </c>
+      <c r="D57" s="24" t="s">
+        <v>241</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="F57" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="G57" s="6" t="s">
-        <v>218</v>
-      </c>
+        <v>242</v>
+      </c>
+      <c r="F57" s="9"/>
+      <c r="G57" s="6"/>
       <c r="H57" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>10</v>
@@ -3097,408 +3134,412 @@
         <v>27</v>
       </c>
       <c r="D58" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="E58" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="E58" s="9" t="s">
-        <v>182</v>
-      </c>
       <c r="F58" s="9" t="s">
-        <v>203</v>
+        <v>159</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="H58" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>184</v>
+        <v>130</v>
       </c>
       <c r="F59" s="9" t="s">
-        <v>161</v>
+        <v>202</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="H59" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B60" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="F60" s="6" t="s">
-        <v>127</v>
+        <v>179</v>
+      </c>
+      <c r="F60" s="9" t="s">
+        <v>198</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>221</v>
+        <v>204</v>
       </c>
       <c r="H60" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B61" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B61" s="23" t="s">
         <v>10</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D61" s="8" t="s">
-        <v>197</v>
+        <v>249</v>
+      </c>
+      <c r="D61" s="24" t="s">
+        <v>243</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="H61" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B62" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>140</v>
+        <v>180</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="F62" s="9"/>
+        <v>181</v>
+      </c>
+      <c r="F62" s="9" t="s">
+        <v>159</v>
+      </c>
       <c r="G62" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H62" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>198</v>
+        <v>169</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="F63" s="6"/>
+        <v>170</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>125</v>
+      </c>
       <c r="G63" s="6" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="H63" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B64" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>175</v>
+        <v>192</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>188</v>
+        <v>130</v>
       </c>
       <c r="F64" s="9" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="H64" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B65" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>175</v>
+        <v>138</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="F65" s="9" t="s">
-        <v>199</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="F65" s="9"/>
       <c r="G65" s="6" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B66" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>138</v>
+        <v>193</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="F66" s="9"/>
+        <v>130</v>
+      </c>
+      <c r="F66" s="6"/>
       <c r="G66" s="6" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="H66" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B67" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D67" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="E67" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="E67" s="9" t="s">
-        <v>186</v>
-      </c>
       <c r="F67" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="G67" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="G67" s="6" t="s">
-        <v>209</v>
-      </c>
       <c r="H67" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B68" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B68" s="23" t="s">
         <v>10</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D68" s="8" t="s">
-        <v>178</v>
+        <v>250</v>
+      </c>
+      <c r="D68" s="24" t="s">
+        <v>244</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="F68" s="9" t="s">
-        <v>201</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="F68" s="6"/>
       <c r="G68" s="6" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="H68" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B69" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>138</v>
+        <v>173</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="F69" s="9"/>
+        <v>185</v>
+      </c>
+      <c r="F69" s="9" t="s">
+        <v>194</v>
+      </c>
       <c r="G69" s="6" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="H69" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B70" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F70" s="9"/>
       <c r="G70" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H70" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B71" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B71" s="23" t="s">
         <v>10</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D71" s="8" t="s">
-        <v>173</v>
+        <v>251</v>
+      </c>
+      <c r="D71" s="24" t="s">
+        <v>245</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F71" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="H71" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="H72" s="1" t="s">
-        <v>110</v>
+      <c r="A72" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D72" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="E72" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="F72" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="G72" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H72" s="6" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>134</v>
+        <v>176</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="F73" s="6"/>
+        <v>175</v>
+      </c>
+      <c r="F73" s="9" t="s">
+        <v>196</v>
+      </c>
       <c r="G73" s="6" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="D74" s="8" t="s">
         <v>136</v>
@@ -3506,275 +3547,454 @@
       <c r="E74" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="F74" s="6"/>
+      <c r="F74" s="9"/>
       <c r="G74" s="6" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="H74" s="6" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D75" s="5" t="s">
+      <c r="A75" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D75" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="E75" s="2" t="s">
+      <c r="E75" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="F75" s="1"/>
-      <c r="G75" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="H75" s="1" t="s">
-        <v>111</v>
+      <c r="F75" s="9"/>
+      <c r="G75" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="H75" s="6" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="G76" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="H76" s="1" t="s">
-        <v>111</v>
+      <c r="A76" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D76" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="F76" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="G76" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="H76" s="6" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>159</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>72</v>
+        <v>115</v>
+      </c>
+      <c r="B78" s="23" t="s">
+        <v>47</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D78" s="8" t="s">
-        <v>148</v>
+        <v>252</v>
+      </c>
+      <c r="D78" s="24" t="s">
+        <v>239</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="F78" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="G78" s="6" t="s">
-        <v>209</v>
-      </c>
+        <v>240</v>
+      </c>
+      <c r="F78" s="6"/>
+      <c r="G78" s="6"/>
       <c r="H78" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B79" s="6" t="s">
-        <v>72</v>
+        <v>115</v>
+      </c>
+      <c r="B79" s="23" t="s">
+        <v>47</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D79" s="8" t="s">
-        <v>151</v>
+        <v>253</v>
+      </c>
+      <c r="D79" s="24" t="s">
+        <v>238</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="F79" s="6" t="s">
-        <v>163</v>
+        <v>203</v>
       </c>
       <c r="G79" s="6" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="H79" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B80" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="E80" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="F80" s="6"/>
+      <c r="G80" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="H80" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D81" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E81" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="F81" s="6"/>
+      <c r="G81" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H81" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F82" s="1"/>
+      <c r="G82" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D85" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="E85" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="F85" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G85" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H85" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D86" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="E86" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="F86" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="G86" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H86" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C87" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C80" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D80" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="E80" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="F80" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="G80" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="H80" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="81" spans="7:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="G81" s="3"/>
-    </row>
-    <row r="82" spans="7:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="G82" s="3"/>
-    </row>
-    <row r="83" spans="7:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="G83" s="3"/>
-    </row>
-    <row r="84" spans="7:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="G84" s="3"/>
-    </row>
-    <row r="85" spans="7:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="G85" s="3"/>
-    </row>
-    <row r="86" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G86" s="1"/>
-    </row>
-    <row r="87" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G87" s="1"/>
+      <c r="D87" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="E87" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="F87" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="G87" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H87" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G88" s="3"/>
+    </row>
+    <row r="89" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G89" s="3"/>
+    </row>
+    <row r="90" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G90" s="3"/>
+    </row>
+    <row r="91" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G91" s="3"/>
+    </row>
+    <row r="92" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G92" s="3"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G93" s="1"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G94" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="A7:H80">
-    <sortCondition ref="A7:A80"/>
-    <sortCondition ref="B7:B80"/>
-    <sortCondition ref="C7:C80"/>
+  <sortState ref="A7:H87">
+    <sortCondition ref="A7:A87"/>
+    <sortCondition ref="B7:B87"/>
+    <sortCondition ref="C7:C87"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="D63" r:id="rId1" tooltip="Show report for KT944306.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KT944306.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{B3076DCA-0B99-8340-8ED6-E5157A2E0AF5}"/>
-    <hyperlink ref="D61" r:id="rId2" tooltip="Show report for XM_015801862.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/XM_015801862.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{088DCC99-EDA0-0241-BDED-09B1CD11E21F}"/>
-    <hyperlink ref="D49" r:id="rId3" tooltip="Show report for HQ906659.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/HQ906659.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{CD78ADC7-2C34-6940-8082-C4E0CE50334A}"/>
-    <hyperlink ref="D57" r:id="rId4" tooltip="Show report for XM_015799557.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/XM_015799557.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{124764B5-49DA-4349-AF34-0850354755F2}"/>
-    <hyperlink ref="D56" r:id="rId5" tooltip="Show report for BK010874.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/BK010874.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{0A4919B2-455F-1440-8E8D-33E5AEAE9BE4}"/>
-    <hyperlink ref="D51" r:id="rId6" tooltip="Show report for XM_015802553.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/XM_015802553.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{98168E9A-9056-BA4F-8EF4-BBFA802F4D2C}"/>
-    <hyperlink ref="D62" r:id="rId7" tooltip="Show report for Y00055.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/Y00055.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{B8995333-7F0B-6546-8074-92C1F19DC637}"/>
-    <hyperlink ref="D52" r:id="rId8" tooltip="Show report for XM_015802462.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/XM_015802462.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{57275589-40BF-BE4F-92CF-3BE62D8FB3DD}"/>
-    <hyperlink ref="D66" r:id="rId9" tooltip="Show report for KT944307.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KT944307.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{9BF3EAE0-2DD2-3743-BFF2-6CF7D0BC5895}"/>
-    <hyperlink ref="D59" r:id="rId10" tooltip="Show report for HQ107970.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/HQ107970.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{DAD46463-5C49-9749-A3C6-34498125B594}"/>
-    <hyperlink ref="D65" r:id="rId11" tooltip="Show report for KT728396.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KT728396.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{F33C9490-0D54-674E-B827-F1F439848D76}"/>
-    <hyperlink ref="D54" r:id="rId12" tooltip="Show report for KT728402.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KT728402.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{168ABCE6-8448-0549-9BB2-EEC5E90E647D}"/>
-    <hyperlink ref="D48" r:id="rId13" tooltip="Show report for KT728394.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KT728394.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{416824ED-F003-EB40-A1AD-B7419F6B2470}"/>
-    <hyperlink ref="D67" r:id="rId14" tooltip="Show report for AB828159.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/AB828159.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{E17E0B0A-6F2F-3045-BEA7-E6563D0D6E60}"/>
-    <hyperlink ref="D55" r:id="rId15" tooltip="Show report for HQ107970.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/HQ107970.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{D62C99A4-BD0F-474A-8C4A-B6871174BABF}"/>
-    <hyperlink ref="D58" r:id="rId16" tooltip="Show report for MK516192.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/MK516192.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{CF6BB84D-8CF3-4643-BDCC-937890D7A90F}"/>
-    <hyperlink ref="D45" r:id="rId17" tooltip="Show report for CP015675.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/CP015675.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{C93244A8-C77E-B44D-A9E8-86C01ABE5658}"/>
-    <hyperlink ref="D47" r:id="rId18" tooltip="Show report for JN006842.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/JN006842.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{B2CBAAB2-6CB3-8648-A944-9E35B63A755B}"/>
-    <hyperlink ref="D53" r:id="rId19" tooltip="Show report for JN006843.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/JN006843.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{2BF9AD94-7673-8C4D-B7FC-242E917BE1C7}"/>
-    <hyperlink ref="D68" r:id="rId20" tooltip="Show report for MN244156.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/MN244156.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{BFA91E5C-EBA2-A244-A593-D705C2668EDE}"/>
-    <hyperlink ref="D70" r:id="rId21" tooltip="Show report for Y00055.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/Y00055.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{67FD4496-0279-4F4B-8BB0-FE18EE055417}"/>
-    <hyperlink ref="D50" r:id="rId22" tooltip="Show report for XM_029023350.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/XM_029023350.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{2A058E16-4B99-504E-A472-9C8F8FDDD3A5}"/>
-    <hyperlink ref="D44" r:id="rId23" tooltip="Show report for Y00055.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/Y00055.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{D2DE8704-5DED-F742-ABF6-6C844D5BAF78}"/>
-    <hyperlink ref="D69" r:id="rId24" tooltip="Show report for KT944307.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KT944307.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{4DE35FC0-48F8-9447-B458-97FEA4D91647}"/>
-    <hyperlink ref="D64" r:id="rId25" tooltip="Show report for KT728396.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KT728396.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{DF4DECB8-8A93-EE49-946D-A87A79363170}"/>
-    <hyperlink ref="D46" r:id="rId26" tooltip="Show report for KT944307.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KT944307.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{94FB1BFA-0316-654E-877B-A5215248C4C7}"/>
-    <hyperlink ref="D71" r:id="rId27" tooltip="Show report for CP015657.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/CP015657.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{4FE5677F-8509-2840-9A24-580F7FDC7EAB}"/>
-    <hyperlink ref="D60" r:id="rId28" tooltip="Show report for CP029526.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/CP029526.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{CA01DBB6-580B-4744-9A60-94ED55C19278}"/>
-    <hyperlink ref="D72" r:id="rId29" tooltip="Show report for KF963538.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KF963538.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{D2AAD6D8-38EB-8B4C-9B31-AADB2729002C}"/>
-    <hyperlink ref="D41" r:id="rId30" tooltip="Show report for AB362411.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/AB362411.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{9F3AD804-71B2-0744-8FBD-4048DCB3EEA9}"/>
-    <hyperlink ref="D43" r:id="rId31" tooltip="Show report for AB828157.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/AB828157.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{73783384-954B-6C42-971F-4E762B98672E}"/>
-    <hyperlink ref="D39" r:id="rId32" tooltip="Show report for JN006847.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/JN006847.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{AD3E45F8-48B2-0847-951B-1399A1AFDB5A}"/>
-    <hyperlink ref="D40" r:id="rId33" tooltip="Show report for AB362411.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/AB362411.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{22E16D7D-B2D5-F14C-BF02-1A7B25387809}"/>
-    <hyperlink ref="D42" r:id="rId34" tooltip="Show report for AJ223562.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/AJ223562.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{EF03B7C0-9C79-F743-B997-D2C4C5010586}"/>
-    <hyperlink ref="D38" r:id="rId35" tooltip="Show report for JF778738.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/JF778738.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{9E1F227D-C3A9-EC4E-9F95-95B1F37519C2}"/>
-    <hyperlink ref="D34" r:id="rId36" tooltip="Show report for AB362411.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/AB362411.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{9DD67234-6C54-9F47-9FC0-A5DA3E49388F}"/>
-    <hyperlink ref="D37" r:id="rId37" tooltip="Show report for JN006849.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/JN006849.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{7A157FA7-157C-AE49-A240-3B6D6CBD1A67}"/>
-    <hyperlink ref="D35" r:id="rId38" tooltip="Show report for AJ223562.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/AJ223562.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{0F157639-70FA-1845-926B-664806AFBFD4}"/>
-    <hyperlink ref="D36" r:id="rId39" tooltip="Show report for AB362411.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/AB362411.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{D4EB364E-4E93-D945-89EB-A3FEBF4D4D7B}"/>
-    <hyperlink ref="D79" r:id="rId40" tooltip="Show report for JN006843.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/JN006843.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{DA9DF788-1AD6-5342-A00A-5164AA304946}"/>
-    <hyperlink ref="D80" r:id="rId41" tooltip="Show report for JN006832.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/JN006832.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{7543871E-B09F-A04A-A517-148CD92ECFCF}"/>
-    <hyperlink ref="D78" r:id="rId42" tooltip="Show report for JN006830.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/JN006830.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{23BA3410-695C-154D-BEF9-E30E309D9F03}"/>
-    <hyperlink ref="D19" r:id="rId43" tooltip="Show report for KF963538.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KF963538.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{4CA6C5DA-87CF-4641-A7E8-224EF1113270}"/>
-    <hyperlink ref="D22" r:id="rId44" tooltip="Show report for KF963538.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KF963538.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{F74B3227-5999-A442-AC49-379F3E379CAC}"/>
-    <hyperlink ref="D21" r:id="rId45" tooltip="Show report for KF963538.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KF963538.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{30133E3E-CD9B-814C-A50F-FA34A9C71019}"/>
-    <hyperlink ref="D20" r:id="rId46" tooltip="Show report for KF963538.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KF963538.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{4E6F91E6-A77B-834D-86C0-784AACC17D66}"/>
-    <hyperlink ref="D18" r:id="rId47" tooltip="Show report for KF963538.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KF963538.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{64E79AD6-26A1-154E-95A6-8B323C738133}"/>
-    <hyperlink ref="D17" r:id="rId48" tooltip="Show report for KF963538.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KF963538.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{4FCD613D-AC0C-1443-BE88-DC9398638779}"/>
-    <hyperlink ref="D77" r:id="rId49" tooltip="Show report for CP040155.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/CP040155.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{2535EE8D-AA55-E942-B32F-10A132276D11}"/>
-    <hyperlink ref="D75" r:id="rId50" tooltip="Show report for KT944307.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KT944307.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{FDE8D65C-B3D2-7641-AD41-1F90251CDEDC}"/>
-    <hyperlink ref="D76" r:id="rId51" tooltip="Show report for KF054114.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KF054114.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{9CFE631C-FC2C-8C41-9A07-D42917047197}"/>
-    <hyperlink ref="D24" r:id="rId52" tooltip="Show report for AF063022.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/AF063022.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{9E514544-7AB9-364C-8D47-00DC713039E0}"/>
-    <hyperlink ref="D23" r:id="rId53" tooltip="Show report for KF963538.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KF963538.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{5FF9D442-6ADD-9A48-8868-3C3A225B2CF4}"/>
-    <hyperlink ref="D28" r:id="rId54" tooltip="Show report for CP040159.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/CP040159.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{3FCF7F79-2C58-EC4A-80FA-790C99EA9310}"/>
-    <hyperlink ref="D25" r:id="rId55" tooltip="Show report for Y00055.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/Y00055.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{B23421E5-6609-3F4C-A550-BF3BA2FDE7E9}"/>
-    <hyperlink ref="D26" r:id="rId56" tooltip="Show report for JN036654.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/JN036654.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{062AFC3E-2146-8640-B453-8C77420E4A6A}"/>
-    <hyperlink ref="D27" r:id="rId57" tooltip="Show report for KT944307.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KT944307.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{B006BCEA-CA24-A742-B966-8EAA9EB86A12}"/>
-    <hyperlink ref="D74" r:id="rId58" tooltip="Show report for FJ807258.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/FJ807258.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{25D539CD-8686-7948-9B42-683C42ACBD9E}"/>
-    <hyperlink ref="D73" r:id="rId59" tooltip="Show report for KY264930.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KY264930.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{A61FFD27-BFD2-1540-9CE4-3B9A6CEC3D60}"/>
-    <hyperlink ref="D33" r:id="rId60" tooltip="Show report for XM_015802891.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/XM_015802891.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{12428869-0254-1247-BB1E-551C846D80F5}"/>
-    <hyperlink ref="D30" r:id="rId61" tooltip="Show report for XM_015800899.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/XM_015800899.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{A60E5A5D-81D0-284A-A318-79FDF0981D72}"/>
-    <hyperlink ref="D31" r:id="rId62" tooltip="Show report for LR697136.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/LR697136.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{A8037CA9-E3C9-E349-ADAF-ECFFF65B2B51}"/>
-    <hyperlink ref="D29" r:id="rId63" tooltip="Show report for KF963538.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KF963538.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{B8A59C23-504B-CD44-A2F9-E3F890FD74AC}"/>
-    <hyperlink ref="D32" r:id="rId64" tooltip="Show report for JN036654.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/JN036654.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{A3733512-620C-B044-877F-F0F2CE1A438F}"/>
-    <hyperlink ref="D10" r:id="rId65" tooltip="Show report for KJ767188.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KJ767188.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNMXDE014" xr:uid="{82B32E93-2F26-284D-B764-042E532D83E7}"/>
-    <hyperlink ref="D9" r:id="rId66" tooltip="Show report for XR_003297360.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/XR_003297360.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNMXDE014" xr:uid="{B85742A8-AC25-9A4D-9887-32986A7F3EFE}"/>
-    <hyperlink ref="D8" r:id="rId67" tooltip="Show report for GU593706.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/GU593706.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNMXDE014" xr:uid="{CD2134AA-821B-C249-9347-2CFA8E452FE9}"/>
-    <hyperlink ref="D7" r:id="rId68" tooltip="Show report for AY625607.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/AY625607.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNMXDE014" xr:uid="{6D1D1B82-4292-5A4C-A52E-689F20928EB6}"/>
-    <hyperlink ref="D15" r:id="rId69" tooltip="Show report for AF245279.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/AF245279.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNMXDE014" xr:uid="{931EEC99-8D45-C147-B90D-A93C1E9BF8E6}"/>
-    <hyperlink ref="D16" r:id="rId70" tooltip="Show report for MH618774.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/MH618774.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNMXDE014" xr:uid="{B22E031B-3C7D-0B4A-828D-96360268A125}"/>
-    <hyperlink ref="D13" r:id="rId71" tooltip="Show report for LN835300.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/LN835300.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNMXDE014" xr:uid="{AFC741B8-B69A-6946-BD05-A62AAFC51C2C}"/>
-    <hyperlink ref="D11" r:id="rId72" tooltip="Show report for KF297603.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KF297603.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNMXDE014" xr:uid="{020ED577-FE69-9848-99A4-5894A1BEA2CF}"/>
-    <hyperlink ref="D14" r:id="rId73" tooltip="Show report for MK650492.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/MK650492.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNMXDE014" xr:uid="{EEB48A2B-952E-BE4F-944C-2CBBAEBFBD7D}"/>
-    <hyperlink ref="D12" r:id="rId74" tooltip="Show report for XR_003699200.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/XR_003699200.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNMXDE014" xr:uid="{05FE3670-4AC1-DE42-A2C6-FB32A66BB0DD}"/>
-    <hyperlink ref="D2" r:id="rId75" tooltip="Show report for KF296322.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KF296322.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2JCEWFJM01N" xr:uid="{DA572C18-00A2-D24A-BBC9-F9C96883DE41}"/>
-    <hyperlink ref="D3" r:id="rId76" tooltip="Show report for MH801203.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/MH801203.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2JCEWFJM01N" xr:uid="{7A365384-AF8B-444D-98B2-2DA8B1093C55}"/>
-    <hyperlink ref="D4" r:id="rId77" tooltip="Show report for KF296328.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KF296328.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2JCEWFJM01N" xr:uid="{8CA1CFA6-FD52-6442-AACF-6F44F8BD2607}"/>
-    <hyperlink ref="D5" r:id="rId78" tooltip="Show report for KF296327.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KF296327.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2JCEWFJM01N" xr:uid="{E2223AF9-B1F5-244F-BB2C-9F0B959A8BD6}"/>
-    <hyperlink ref="D6" r:id="rId79" tooltip="Show report for KF296331.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KF296331.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2JCEWFJM01N" xr:uid="{19A24EDC-A870-064D-AB20-B5638F731F6C}"/>
+    <hyperlink ref="D66" r:id="rId1" tooltip="Show report for KT944306.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KT944306.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{B3076DCA-0B99-8340-8ED6-E5157A2E0AF5}"/>
+    <hyperlink ref="D64" r:id="rId2" tooltip="Show report for XM_015801862.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/XM_015801862.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{088DCC99-EDA0-0241-BDED-09B1CD11E21F}"/>
+    <hyperlink ref="D51" r:id="rId3" tooltip="Show report for HQ906659.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/HQ906659.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{CD78ADC7-2C34-6940-8082-C4E0CE50334A}"/>
+    <hyperlink ref="D59" r:id="rId4" tooltip="Show report for XM_015799557.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/XM_015799557.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{124764B5-49DA-4349-AF34-0850354755F2}"/>
+    <hyperlink ref="D53" r:id="rId5" tooltip="Show report for XM_015802553.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/XM_015802553.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{98168E9A-9056-BA4F-8EF4-BBFA802F4D2C}"/>
+    <hyperlink ref="D65" r:id="rId6" tooltip="Show report for Y00055.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/Y00055.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{B8995333-7F0B-6546-8074-92C1F19DC637}"/>
+    <hyperlink ref="D54" r:id="rId7" tooltip="Show report for XM_015802462.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/XM_015802462.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{57275589-40BF-BE4F-92CF-3BE62D8FB3DD}"/>
+    <hyperlink ref="D70" r:id="rId8" tooltip="Show report for KT944307.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KT944307.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{9BF3EAE0-2DD2-3743-BFF2-6CF7D0BC5895}"/>
+    <hyperlink ref="D62" r:id="rId9" tooltip="Show report for HQ107970.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/HQ107970.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{DAD46463-5C49-9749-A3C6-34498125B594}"/>
+    <hyperlink ref="D69" r:id="rId10" tooltip="Show report for KT728396.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KT728396.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{F33C9490-0D54-674E-B827-F1F439848D76}"/>
+    <hyperlink ref="D56" r:id="rId11" tooltip="Show report for KT728402.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KT728402.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{168ABCE6-8448-0549-9BB2-EEC5E90E647D}"/>
+    <hyperlink ref="D50" r:id="rId12" tooltip="Show report for KT728394.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KT728394.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{416824ED-F003-EB40-A1AD-B7419F6B2470}"/>
+    <hyperlink ref="D72" r:id="rId13" tooltip="Show report for AB828159.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/AB828159.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{E17E0B0A-6F2F-3045-BEA7-E6563D0D6E60}"/>
+    <hyperlink ref="D58" r:id="rId14" tooltip="Show report for HQ107970.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/HQ107970.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{D62C99A4-BD0F-474A-8C4A-B6871174BABF}"/>
+    <hyperlink ref="D60" r:id="rId15" tooltip="Show report for MK516192.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/MK516192.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{CF6BB84D-8CF3-4643-BDCC-937890D7A90F}"/>
+    <hyperlink ref="D49" r:id="rId16" tooltip="Show report for JN006842.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/JN006842.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{B2CBAAB2-6CB3-8648-A944-9E35B63A755B}"/>
+    <hyperlink ref="D55" r:id="rId17" tooltip="Show report for JN006843.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/JN006843.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{2BF9AD94-7673-8C4D-B7FC-242E917BE1C7}"/>
+    <hyperlink ref="D73" r:id="rId18" tooltip="Show report for MN244156.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/MN244156.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{BFA91E5C-EBA2-A244-A593-D705C2668EDE}"/>
+    <hyperlink ref="D75" r:id="rId19" tooltip="Show report for Y00055.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/Y00055.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{67FD4496-0279-4F4B-8BB0-FE18EE055417}"/>
+    <hyperlink ref="D52" r:id="rId20" tooltip="Show report for XM_029023350.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/XM_029023350.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{2A058E16-4B99-504E-A472-9C8F8FDDD3A5}"/>
+    <hyperlink ref="D47" r:id="rId21" tooltip="Show report for Y00055.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/Y00055.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{D2DE8704-5DED-F742-ABF6-6C844D5BAF78}"/>
+    <hyperlink ref="D74" r:id="rId22" tooltip="Show report for KT944307.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KT944307.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{4DE35FC0-48F8-9447-B458-97FEA4D91647}"/>
+    <hyperlink ref="D67" r:id="rId23" tooltip="Show report for KT728396.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KT728396.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{DF4DECB8-8A93-EE49-946D-A87A79363170}"/>
+    <hyperlink ref="D48" r:id="rId24" tooltip="Show report for KT944307.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KT944307.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{94FB1BFA-0316-654E-877B-A5215248C4C7}"/>
+    <hyperlink ref="D76" r:id="rId25" tooltip="Show report for CP015657.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/CP015657.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{4FE5677F-8509-2840-9A24-580F7FDC7EAB}"/>
+    <hyperlink ref="D63" r:id="rId26" tooltip="Show report for CP029526.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/CP029526.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2EV5AYAF016" xr:uid="{CA01DBB6-580B-4744-9A60-94ED55C19278}"/>
+    <hyperlink ref="D77" r:id="rId27" tooltip="Show report for KF963538.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KF963538.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{D2AAD6D8-38EB-8B4C-9B31-AADB2729002C}"/>
+    <hyperlink ref="D44" r:id="rId28" tooltip="Show report for AB362411.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/AB362411.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{9F3AD804-71B2-0744-8FBD-4048DCB3EEA9}"/>
+    <hyperlink ref="D46" r:id="rId29" tooltip="Show report for AB828157.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/AB828157.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{73783384-954B-6C42-971F-4E762B98672E}"/>
+    <hyperlink ref="D42" r:id="rId30" tooltip="Show report for JN006847.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/JN006847.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{AD3E45F8-48B2-0847-951B-1399A1AFDB5A}"/>
+    <hyperlink ref="D43" r:id="rId31" tooltip="Show report for AB362411.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/AB362411.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{22E16D7D-B2D5-F14C-BF02-1A7B25387809}"/>
+    <hyperlink ref="D45" r:id="rId32" tooltip="Show report for AJ223562.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/AJ223562.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{EF03B7C0-9C79-F743-B997-D2C4C5010586}"/>
+    <hyperlink ref="D41" r:id="rId33" tooltip="Show report for JF778738.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/JF778738.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{9E1F227D-C3A9-EC4E-9F95-95B1F37519C2}"/>
+    <hyperlink ref="D37" r:id="rId34" tooltip="Show report for AB362411.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/AB362411.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{9DD67234-6C54-9F47-9FC0-A5DA3E49388F}"/>
+    <hyperlink ref="D40" r:id="rId35" tooltip="Show report for JN006849.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/JN006849.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{7A157FA7-157C-AE49-A240-3B6D6CBD1A67}"/>
+    <hyperlink ref="D38" r:id="rId36" tooltip="Show report for AJ223562.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/AJ223562.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{0F157639-70FA-1845-926B-664806AFBFD4}"/>
+    <hyperlink ref="D39" r:id="rId37" tooltip="Show report for AB362411.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/AB362411.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{D4EB364E-4E93-D945-89EB-A3FEBF4D4D7B}"/>
+    <hyperlink ref="D86" r:id="rId38" tooltip="Show report for JN006843.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/JN006843.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{DA9DF788-1AD6-5342-A00A-5164AA304946}"/>
+    <hyperlink ref="D87" r:id="rId39" tooltip="Show report for JN006832.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/JN006832.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{7543871E-B09F-A04A-A517-148CD92ECFCF}"/>
+    <hyperlink ref="D85" r:id="rId40" tooltip="Show report for JN006830.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/JN006830.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{23BA3410-695C-154D-BEF9-E30E309D9F03}"/>
+    <hyperlink ref="D19" r:id="rId41" tooltip="Show report for KF963538.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KF963538.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{4CA6C5DA-87CF-4641-A7E8-224EF1113270}"/>
+    <hyperlink ref="D22" r:id="rId42" tooltip="Show report for KF963538.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KF963538.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{F74B3227-5999-A442-AC49-379F3E379CAC}"/>
+    <hyperlink ref="D21" r:id="rId43" tooltip="Show report for KF963538.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KF963538.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{30133E3E-CD9B-814C-A50F-FA34A9C71019}"/>
+    <hyperlink ref="D20" r:id="rId44" tooltip="Show report for KF963538.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KF963538.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{4E6F91E6-A77B-834D-86C0-784AACC17D66}"/>
+    <hyperlink ref="D18" r:id="rId45" tooltip="Show report for KF963538.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KF963538.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{64E79AD6-26A1-154E-95A6-8B323C738133}"/>
+    <hyperlink ref="D17" r:id="rId46" tooltip="Show report for KF963538.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KF963538.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{4FCD613D-AC0C-1443-BE88-DC9398638779}"/>
+    <hyperlink ref="D84" r:id="rId47" tooltip="Show report for CP040155.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/CP040155.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{2535EE8D-AA55-E942-B32F-10A132276D11}"/>
+    <hyperlink ref="D82" r:id="rId48" tooltip="Show report for KT944307.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KT944307.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{FDE8D65C-B3D2-7641-AD41-1F90251CDEDC}"/>
+    <hyperlink ref="D83" r:id="rId49" tooltip="Show report for KF054114.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KF054114.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{9CFE631C-FC2C-8C41-9A07-D42917047197}"/>
+    <hyperlink ref="D25" r:id="rId50" tooltip="Show report for AF063022.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/AF063022.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{9E514544-7AB9-364C-8D47-00DC713039E0}"/>
+    <hyperlink ref="D23" r:id="rId51" tooltip="Show report for KF963538.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KF963538.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{5FF9D442-6ADD-9A48-8868-3C3A225B2CF4}"/>
+    <hyperlink ref="D29" r:id="rId52" tooltip="Show report for CP040159.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/CP040159.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{3FCF7F79-2C58-EC4A-80FA-790C99EA9310}"/>
+    <hyperlink ref="D26" r:id="rId53" tooltip="Show report for Y00055.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/Y00055.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{B23421E5-6609-3F4C-A550-BF3BA2FDE7E9}"/>
+    <hyperlink ref="D27" r:id="rId54" tooltip="Show report for JN036654.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/JN036654.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{062AFC3E-2146-8640-B453-8C77420E4A6A}"/>
+    <hyperlink ref="D28" r:id="rId55" tooltip="Show report for KT944307.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KT944307.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{B006BCEA-CA24-A742-B966-8EAA9EB86A12}"/>
+    <hyperlink ref="D81" r:id="rId56" tooltip="Show report for FJ807258.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/FJ807258.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{25D539CD-8686-7948-9B42-683C42ACBD9E}"/>
+    <hyperlink ref="D80" r:id="rId57" tooltip="Show report for KY264930.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KY264930.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{A61FFD27-BFD2-1540-9CE4-3B9A6CEC3D60}"/>
+    <hyperlink ref="D35" r:id="rId58" tooltip="Show report for XM_015802891.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/XM_015802891.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{12428869-0254-1247-BB1E-551C846D80F5}"/>
+    <hyperlink ref="D31" r:id="rId59" tooltip="Show report for XM_015800899.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/XM_015800899.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{A60E5A5D-81D0-284A-A318-79FDF0981D72}"/>
+    <hyperlink ref="D32" r:id="rId60" tooltip="Show report for LR697136.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/LR697136.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{A8037CA9-E3C9-E349-ADAF-ECFFF65B2B51}"/>
+    <hyperlink ref="D30" r:id="rId61" tooltip="Show report for KF963538.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KF963538.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{B8A59C23-504B-CD44-A2F9-E3F890FD74AC}"/>
+    <hyperlink ref="D34" r:id="rId62" tooltip="Show report for JN036654.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/JN036654.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNZ7MP014" xr:uid="{A3733512-620C-B044-877F-F0F2CE1A438F}"/>
+    <hyperlink ref="D10" r:id="rId63" tooltip="Show report for KJ767188.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KJ767188.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNMXDE014" xr:uid="{82B32E93-2F26-284D-B764-042E532D83E7}"/>
+    <hyperlink ref="D9" r:id="rId64" tooltip="Show report for XR_003297360.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/XR_003297360.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNMXDE014" xr:uid="{B85742A8-AC25-9A4D-9887-32986A7F3EFE}"/>
+    <hyperlink ref="D8" r:id="rId65" tooltip="Show report for GU593706.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/GU593706.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNMXDE014" xr:uid="{CD2134AA-821B-C249-9347-2CFA8E452FE9}"/>
+    <hyperlink ref="D7" r:id="rId66" tooltip="Show report for AY625607.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/AY625607.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNMXDE014" xr:uid="{6D1D1B82-4292-5A4C-A52E-689F20928EB6}"/>
+    <hyperlink ref="D15" r:id="rId67" tooltip="Show report for AF245279.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/AF245279.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNMXDE014" xr:uid="{931EEC99-8D45-C147-B90D-A93C1E9BF8E6}"/>
+    <hyperlink ref="D16" r:id="rId68" tooltip="Show report for MH618774.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/MH618774.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNMXDE014" xr:uid="{B22E031B-3C7D-0B4A-828D-96360268A125}"/>
+    <hyperlink ref="D13" r:id="rId69" tooltip="Show report for LN835300.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/LN835300.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNMXDE014" xr:uid="{AFC741B8-B69A-6946-BD05-A62AAFC51C2C}"/>
+    <hyperlink ref="D11" r:id="rId70" tooltip="Show report for KF297603.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KF297603.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNMXDE014" xr:uid="{020ED577-FE69-9848-99A4-5894A1BEA2CF}"/>
+    <hyperlink ref="D14" r:id="rId71" tooltip="Show report for MK650492.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/MK650492.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNMXDE014" xr:uid="{EEB48A2B-952E-BE4F-944C-2CBBAEBFBD7D}"/>
+    <hyperlink ref="D12" r:id="rId72" tooltip="Show report for XR_003699200.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/XR_003699200.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2CDNMXDE014" xr:uid="{05FE3670-4AC1-DE42-A2C6-FB32A66BB0DD}"/>
+    <hyperlink ref="D2" r:id="rId73" tooltip="Show report for KF296322.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KF296322.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2JCEWFJM01N" xr:uid="{DA572C18-00A2-D24A-BBC9-F9C96883DE41}"/>
+    <hyperlink ref="D3" r:id="rId74" tooltip="Show report for MH801203.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/MH801203.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2JCEWFJM01N" xr:uid="{7A365384-AF8B-444D-98B2-2DA8B1093C55}"/>
+    <hyperlink ref="D4" r:id="rId75" tooltip="Show report for KF296328.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KF296328.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2JCEWFJM01N" xr:uid="{8CA1CFA6-FD52-6442-AACF-6F44F8BD2607}"/>
+    <hyperlink ref="D5" r:id="rId76" tooltip="Show report for KF296327.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KF296327.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2JCEWFJM01N" xr:uid="{E2223AF9-B1F5-244F-BB2C-9F0B959A8BD6}"/>
+    <hyperlink ref="D6" r:id="rId77" tooltip="Show report for KF296331.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KF296331.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=2JCEWFJM01N" xr:uid="{19A24EDC-A870-064D-AB20-B5638F731F6C}"/>
+    <hyperlink ref="D24" r:id="rId78" tooltip="Show report for XM_015805759.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/XM_015805759.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=8PXVPNJY016" xr:uid="{C659A8F1-131B-174C-8A96-3FB8ABD78B5B}"/>
+    <hyperlink ref="D33" r:id="rId79" tooltip="Show report for XM_015796546.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/XM_015796546.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=8PXVPNJY016" xr:uid="{7BAC93BB-438B-284D-9D4F-93AA81C6A648}"/>
+    <hyperlink ref="D36" r:id="rId80" tooltip="Show report for XM_015796549.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/XM_015796549.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=8PXVPNJY016" xr:uid="{3377495A-5CC0-9947-89B2-33B3B4EB8CD7}"/>
+    <hyperlink ref="D79" r:id="rId81" tooltip="Show report for XM_015802014.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/XM_015802014.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=8PXVPNJY016" xr:uid="{FEA233A1-6A2A-F04A-9577-A76BB13691FA}"/>
+    <hyperlink ref="D78" r:id="rId82" tooltip="Show report for KT944293.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/KT944293.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=8PXVPNJY016" xr:uid="{8B3721E0-DD4A-C24D-8E57-CF364F48CE25}"/>
+    <hyperlink ref="D57" r:id="rId83" tooltip="Show report for XM_003877341.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/XM_003877341.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=8PXVPNJY016" xr:uid="{1195FECF-E026-5D4D-9203-3F3DF6067CDD}"/>
+    <hyperlink ref="D61" r:id="rId84" tooltip="Show report for XM_015798305.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/XM_015798305.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=8PXVPNJY016" xr:uid="{F9F5F217-79B5-E64F-A87E-E10C94EB3897}"/>
+    <hyperlink ref="D68" r:id="rId85" tooltip="Show report for XR_001548769.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/XR_001548769.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=8PXVPNJY016" xr:uid="{C74A88C0-FE6E-D146-891B-881B9B8ADFD2}"/>
+    <hyperlink ref="D71" r:id="rId86" tooltip="Show report for XM_801183.1" display="https://www.ncbi.nlm.nih.gov/nucleotide/XM_801183.1?report=genbank&amp;log$=nucltop&amp;blast_rank=1&amp;RID=8PXVPNJY016" xr:uid="{AD95995C-A60C-564B-938F-727BE0AC52D6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>